<commit_message>
new forms and assets
</commit_message>
<xml_diff>
--- a/xlsx/M&E/indicadores_form_1.xlsx
+++ b/xlsx/M&E/indicadores_form_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Terra_Share\projects\CaVaTeCo_Collect\projects\A_CaVaTeCo_projects\odk_forms_ilrg_lamadi\xlsx\M&amp;E\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CF3157-0F36-479F-AD9D-1BD575E6BD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9E213F-3386-4ECF-B006-9403CD0BBE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="236">
   <si>
     <t>type</t>
   </si>
@@ -707,37 +707,68 @@
     <t>Mulheres e Conselho de Direcção</t>
   </si>
   <si>
+    <t>g8</t>
+  </si>
+  <si>
+    <t>select_one survey_types</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>Isto é o inquérito de linha de base ou o inquérito final?</t>
+  </si>
+  <si>
+    <t>survey_types</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>Inquerito de Linha de Base (inicio)</t>
+  </si>
+  <si>
+    <t>endline</t>
+  </si>
+  <si>
+    <t>Inquerito Final (fim)</t>
+  </si>
+  <si>
+    <t>"LAMADI - Sofala"</t>
+  </si>
+  <si>
+    <t>terrafirma_TN_iTC.jpg</t>
+  </si>
+  <si>
+    <t>search('enum_names_lamadi_sofala', 'startswith', 'enumerator_name', ${searchtext})</t>
+  </si>
+  <si>
+    <t>pulldata('enum_names_lamadi_sofala', 'enumerator_name', 'name_id_key', ${enum_name_id})</t>
+  </si>
+  <si>
+    <t>search('povoado_names_lamadi_sofala', 'matches', 'post_id', ${post_id})</t>
+  </si>
+  <si>
+    <t>pulldata('povoado_names_lamadi_sofala', 'village_name',  'village_id_key', ${village_id})</t>
+  </si>
+  <si>
     <t>http://cavateco.terrafirma.co.mz:8080/lamadi_sofala/submission</t>
-  </si>
-  <si>
-    <t>"LAMADI - Sofala"</t>
-  </si>
-  <si>
-    <t>terrafirma_TN_iTC.jpg</t>
-  </si>
-  <si>
-    <t>search('enum_names_lamadi_sofala', 'startswith', 'enumerator_name', ${searchtext})</t>
-  </si>
-  <si>
-    <t>pulldata('enum_names_lamadi_sofala', 'enumerator_name', 'name_id_key', ${enum_name_id})</t>
-  </si>
-  <si>
-    <t>search('povoado_names_lamadi_sofala', 'matches', 'post_id', ${post_id})</t>
-  </si>
-  <si>
-    <t>pulldata('povoado_names_lamadi_sofala', 'village_name',  'village_id_key', ${village_id})</t>
-  </si>
-  <si>
-    <t>g8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1000,398 +1031,406 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="245">
+  <cellStyleXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="234" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="234" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="233" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="245"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="245" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="245" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="245" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="245" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="245" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="244"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="244" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="244" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="244" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="244" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="244" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="244" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="245">
+  <cellStyles count="246">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1624,6 +1663,7 @@
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="233" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
     <cellStyle name="Normal 3" xfId="243" xr:uid="{F27830CB-79FD-41FE-957A-3C449CF5F143}"/>
@@ -1636,7 +1676,7 @@
     <cellStyle name="Normal 3 2 2 2 4 2" xfId="240" xr:uid="{B8C11DA2-38A1-4072-A7DF-8A4AA610F390}"/>
     <cellStyle name="Normal 3 2 2 2 4 3" xfId="242" xr:uid="{D6C83E32-3598-4E78-815F-583BF3742142}"/>
     <cellStyle name="Normal 3 2 2 2 5" xfId="239" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
-    <cellStyle name="Normal 6" xfId="244" xr:uid="{7A261266-44D5-4E26-A9C8-ECD677CE25A7}"/>
+    <cellStyle name="Normal 6" xfId="245" xr:uid="{7A261266-44D5-4E26-A9C8-ECD677CE25A7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1973,13 +2013,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H46" sqref="H46"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2102,8 +2142,9 @@
         <v>119</v>
       </c>
       <c r="N7" s="55" t="s">
-        <v>221</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="O7" s="70"/>
     </row>
     <row r="8" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -2116,6 +2157,8 @@
       <c r="L8" s="29" t="s">
         <v>61</v>
       </c>
+      <c r="N8" s="70"/>
+      <c r="O8" s="70"/>
     </row>
     <row r="9" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
@@ -2124,8 +2167,9 @@
       <c r="B9" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="O9" s="68" t="s">
-        <v>222</v>
+      <c r="N9" s="70"/>
+      <c r="O9" s="71" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="29" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -2152,55 +2196,55 @@
       <c r="B12" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="66" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58" t="s">
+    <row r="13" spans="1:16" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="57" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="58" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="58" t="s">
+    <row r="14" spans="1:16" s="57" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="60" t="s">
         <v>178</v>
       </c>
-      <c r="D14" s="61"/>
-      <c r="F14" s="62" t="s">
+      <c r="D14" s="60"/>
+      <c r="F14" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="G14" s="62"/>
-      <c r="J14" s="58" t="s">
+      <c r="G14" s="61"/>
+      <c r="J14" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="60" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="58" t="s">
+      <c r="L14" s="59" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="N15" s="60" t="s">
-        <v>224</v>
+      <c r="N15" s="59" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -2280,687 +2324,703 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="56" t="s">
+    <row r="20" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="70" t="s">
         <v>128</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="72" t="s">
         <v>129</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="70" t="s">
         <v>171</v>
       </c>
-      <c r="J20" s="56" t="s">
+      <c r="J20" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="68" t="s">
-        <v>225</v>
-      </c>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-    </row>
-    <row r="21" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58" t="s">
+      <c r="L20" s="71" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="58" t="s">
         <v>169</v>
       </c>
-      <c r="L21" s="60"/>
-      <c r="N21" s="60" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="L21" s="59"/>
+      <c r="N21" s="59" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="J22" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" s="59"/>
+    </row>
+    <row r="23" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B23" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="36" t="s">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B24" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="56" t="s">
+      <c r="C24" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="J23" s="33" t="s">
+      <c r="J24" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="36" t="s">
+      <c r="L24" s="36" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="30"/>
     </row>
     <row r="25" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="30"/>
+    </row>
+    <row r="26" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B26" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G26" s="36" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="J26" s="36" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="36" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
       <c r="J27" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="L27" s="29" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="28" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G28" s="36"/>
       <c r="J28" s="36" t="s">
         <v>20</v>
       </c>
       <c r="L28" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="36"/>
+      <c r="J29" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="L29" s="29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="30"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
+      <c r="B30" s="30"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B31" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C31" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="G30" s="36" t="s">
+      <c r="G31" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="J30" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="34"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="19"/>
       <c r="J31" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="36" t="s">
         <v>109</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" s="34"/>
       <c r="F32" s="16"/>
-      <c r="G32" s="36" t="s">
-        <v>97</v>
-      </c>
+      <c r="G32" s="15"/>
       <c r="H32" s="29"/>
       <c r="I32" s="19"/>
-      <c r="J32" s="36" t="s">
+      <c r="J32" s="16" t="s">
         <v>20</v>
       </c>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
     </row>
-    <row r="33" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="34"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="H33" s="29"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+    </row>
+    <row r="34" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B34" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G33" s="36" t="s">
+      <c r="G34" s="36" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="36" t="s">
+    <row r="35" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B35" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C35" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="J34" s="36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="C35" s="36" t="s">
-        <v>106</v>
-      </c>
       <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
       <c r="J35" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="L35" s="29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="G36" s="36"/>
       <c r="J36" s="36" t="s">
         <v>20</v>
       </c>
       <c r="L36" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" s="36"/>
+      <c r="J37" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" s="29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="30"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
+      <c r="B38" s="30"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B39" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C39" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="G38" s="36" t="s">
+      <c r="G39" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="J38" s="16"/>
-    </row>
-    <row r="39" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="J39" s="16"/>
+    </row>
+    <row r="40" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B40" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="G39" s="66" t="s">
+      <c r="G40" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="L39" s="66" t="s">
+      <c r="L40" s="67" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="66" t="s">
+    <row r="41" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B40" s="67" t="s">
+      <c r="B41" s="68" t="s">
         <v>218</v>
       </c>
-      <c r="C40" s="66" t="s">
+      <c r="C41" s="67" t="s">
         <v>217</v>
       </c>
-      <c r="J40" s="66" t="s">
+      <c r="J41" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L40" s="66" t="s">
+      <c r="L41" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="66" t="s">
+    <row r="42" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B41" s="67" t="s">
+      <c r="B42" s="68" t="s">
         <v>216</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C42" s="67" t="s">
         <v>215</v>
       </c>
-      <c r="J41" s="66" t="s">
+      <c r="J42" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L41" s="66" t="s">
+      <c r="L42" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="66" t="s">
+    <row r="43" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B42" s="67" t="s">
+      <c r="B43" s="68" t="s">
         <v>214</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C43" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="J42" s="66" t="s">
+      <c r="J43" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L42" s="66" t="s">
+      <c r="L43" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="66" t="s">
+    <row r="44" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B43" s="67" t="s">
+      <c r="B44" s="68" t="s">
         <v>212</v>
       </c>
-      <c r="C43" s="66" t="s">
+      <c r="C44" s="67" t="s">
         <v>211</v>
       </c>
-      <c r="J43" s="66" t="s">
+      <c r="J44" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L43" s="66" t="s">
+      <c r="L44" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="66" t="s">
+    <row r="45" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B44" s="67" t="s">
+      <c r="B45" s="68" t="s">
         <v>210</v>
       </c>
-      <c r="C44" s="66" t="s">
+      <c r="C45" s="67" t="s">
         <v>209</v>
       </c>
-      <c r="J44" s="66" t="s">
+      <c r="J45" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L44" s="66" t="s">
+      <c r="L45" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="67"/>
-    </row>
-    <row r="46" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="68"/>
+    </row>
+    <row r="47" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B47" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G46" s="66" t="s">
+      <c r="G47" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="L46" s="66" t="s">
+      <c r="L47" s="67" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="66" t="s">
+    <row r="48" spans="1:13" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B47" s="67" t="s">
+      <c r="B48" s="68" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="66" t="s">
+      <c r="C48" s="67" t="s">
         <v>205</v>
       </c>
-      <c r="J47" s="66" t="s">
+      <c r="J48" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L47" s="66" t="s">
+      <c r="L48" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="66" t="s">
+    <row r="49" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B48" s="67" t="s">
+      <c r="B49" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="C48" s="66" t="s">
+      <c r="C49" s="67" t="s">
         <v>203</v>
       </c>
-      <c r="J48" s="66" t="s">
+      <c r="J49" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L48" s="66" t="s">
+      <c r="L49" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="66" t="s">
+    <row r="50" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B49" s="67" t="s">
+      <c r="B50" s="68" t="s">
         <v>202</v>
       </c>
-      <c r="C49" s="66" t="s">
+      <c r="C50" s="67" t="s">
         <v>201</v>
       </c>
-      <c r="J49" s="66" t="s">
+      <c r="J50" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L49" s="66" t="s">
+      <c r="L50" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="67"/>
-    </row>
-    <row r="51" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="68"/>
+    </row>
+    <row r="52" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B52" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G51" s="66" t="s">
+      <c r="G52" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="L51" s="66" t="s">
+      <c r="L52" s="67" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="66" t="s">
+    <row r="53" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B52" s="67" t="s">
+      <c r="B53" s="68" t="s">
         <v>198</v>
       </c>
-      <c r="C52" s="66" t="s">
+      <c r="C53" s="67" t="s">
         <v>197</v>
       </c>
-      <c r="J52" s="66" t="s">
+      <c r="J53" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L52" s="66" t="s">
+      <c r="L53" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="66" t="s">
+    <row r="54" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B53" s="67" t="s">
+      <c r="B54" s="68" t="s">
         <v>196</v>
       </c>
-      <c r="C53" s="66" t="s">
+      <c r="C54" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="J53" s="66" t="s">
+      <c r="J54" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L53" s="66" t="s">
+      <c r="L54" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="66" t="s">
+    <row r="55" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B54" s="67" t="s">
+      <c r="B55" s="68" t="s">
         <v>194</v>
       </c>
-      <c r="C54" s="66" t="s">
+      <c r="C55" s="67" t="s">
         <v>193</v>
       </c>
-      <c r="J54" s="66" t="s">
+      <c r="J55" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L54" s="66" t="s">
+      <c r="L55" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="67"/>
-    </row>
-    <row r="56" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="66" t="s">
+      <c r="B56" s="68"/>
+    </row>
+    <row r="57" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="B56" s="67" t="s">
+      <c r="B57" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="66" t="s">
+      <c r="C57" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="I56" s="19"/>
-      <c r="J56" s="66" t="s">
+      <c r="I57" s="19"/>
+      <c r="J57" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="L56" s="66" t="s">
+      <c r="L57" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="36" t="s">
+    <row r="58" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B57" s="37" t="s">
+      <c r="B58" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C57" s="36" t="s">
+      <c r="C58" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="G57" s="36" t="s">
+      <c r="G58" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="J57" s="33" t="s">
+      <c r="J58" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="L57" s="36" t="s">
+      <c r="L58" s="36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="15" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B58" s="37" t="s">
+      <c r="B59" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="44" t="s">
+      <c r="C59" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="G58" s="36" t="s">
+      <c r="G59" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="J58" s="16"/>
-    </row>
-    <row r="59" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="J59" s="16"/>
+    </row>
+    <row r="60" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="B60" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="G59" s="66" t="s">
+      <c r="G60" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="L59" s="66" t="s">
+      <c r="L60" s="67" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="66" t="s">
+    <row r="61" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="67" t="s">
         <v>187</v>
       </c>
-      <c r="B60" s="67" t="s">
+      <c r="B61" s="68" t="s">
         <v>189</v>
       </c>
-      <c r="C60" s="66" t="s">
+      <c r="C61" s="67" t="s">
         <v>188</v>
       </c>
-      <c r="J60" s="66" t="s">
+      <c r="J61" s="67" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="66" t="s">
+    <row r="62" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="67" t="s">
         <v>187</v>
       </c>
-      <c r="B61" s="67" t="s">
+      <c r="B62" s="68" t="s">
         <v>186</v>
       </c>
-      <c r="C61" s="66" t="s">
+      <c r="C62" s="67" t="s">
         <v>185</v>
       </c>
-      <c r="J61" s="66" t="s">
+      <c r="J62" s="67" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="67"/>
-    </row>
-    <row r="63" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="36" t="s">
+      <c r="B63" s="68"/>
+    </row>
+    <row r="64" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="37" t="s">
+      <c r="B64" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="C63" s="36" t="s">
+      <c r="C64" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="G63" s="36"/>
-      <c r="J63" s="33" t="s">
+      <c r="G64" s="36"/>
+      <c r="J64" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="L63" s="36" t="s">
+      <c r="L64" s="36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="15" t="s">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="37" t="s">
+      <c r="B65" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C64" s="44" t="s">
+      <c r="C65" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="G64" s="36" t="s">
+      <c r="G65" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="J64" s="16"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
+      <c r="J65" s="16"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B66" s="25" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2972,13 +3032,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3136,7 +3196,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
@@ -3147,7 +3207,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
@@ -3158,7 +3218,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="53" t="s">
         <v>167</v>
       </c>
@@ -3169,21 +3229,51 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="53"/>
       <c r="B21" s="46"/>
       <c r="C21" s="53"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="63" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="63" t="s">
         <v>181</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="C23" s="62" t="s">
         <v>182</v>
       </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="69" t="s">
+        <v>224</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="C27" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="69" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" s="69" t="s">
+        <v>228</v>
+      </c>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -8005,8 +8095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8014,7 +8104,7 @@
     <col min="1" max="1" width="34.69921875" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.3984375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.19921875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="52" style="6" customWidth="1"/>
+    <col min="4" max="4" width="76.8984375" style="6" customWidth="1"/>
     <col min="5" max="5" width="24.5" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="6"/>
   </cols>
@@ -8036,18 +8126,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="68">
-        <v>2022020201</v>
-      </c>
-      <c r="D2" s="68" t="s">
-        <v>220</v>
+      <c r="C2" s="64">
+        <v>2022040601</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>235</v>
       </c>
       <c r="E2" s="44" t="s">
         <v>166</v>
@@ -8061,7 +8151,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{12691883-7B92-40FB-A4A7-E995CA6D1876}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0795315A-7D08-42DA-8289-B68F148FCFA2}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>